<commit_message>
DECLARACIÓN DE ESFUERZO, EXPERIMENTO FINAL 2
</commit_message>
<xml_diff>
--- a/DeclaracionEsfuerzo.xlsx
+++ b/DeclaracionEsfuerzo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.reyesm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCB72F3A-F656-4E1D-9180-F44284466242}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B479DC2-F417-4169-8372-42CC2C91586A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Declaracion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Nota: De acuerdo al programa del curso cada experimento tiene una nota global (en el ejemplo de abajo es B3) y una nota individual (columna K), esta última depende del esfuerzo de cada miembro (columna J). A ese esfuerzo se llega a partir de una reunión de grupo en donde se revisan las contribuciones de cada miembro para poner en funcionamiento cada uno de los puntos de arquitectura. Las celdas B12 a B20 ejemplifican los puntos para el exp. 1. Si el miembro del equipo contribuyó en ese punto de la arquitectura se marca con X. Luego, a partir de las X, el grupo estima el porcentaje de esfuerzo de cada miembro. 
 Se espera que Uds. suban a github un excel similar a este, en donde enuncien el esfuerzo de cada miembro. A partir de allí y la nota global del experimento, el instructor calculará la nota individual. El máximo valor de la nota individual es 5.</t>
@@ -62,22 +62,19 @@
     <t>Michael Osorio</t>
   </si>
   <si>
-    <t>Servicios rest usuarios</t>
-  </si>
-  <si>
-    <t>Autenticacion y Autorización</t>
-  </si>
-  <si>
-    <t>Gestionar horarios de acceso</t>
-  </si>
-  <si>
-    <t>Código EEPROM</t>
-  </si>
-  <si>
-    <t>Gestion de claves de acceso (puerta)</t>
-  </si>
-  <si>
     <t>Arreglos escenario de calidad</t>
+  </si>
+  <si>
+    <t>Extensión endidad física</t>
+  </si>
+  <si>
+    <t>Extensión entidad virtual</t>
+  </si>
+  <si>
+    <t>Seguridad de tópicos</t>
+  </si>
+  <si>
+    <t>HealthChecks y correos de notificación</t>
   </si>
 </sst>
 </file>
@@ -184,11 +181,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,31 +500,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="7" max="7" width="14.42578125" style="12"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -536,9 +529,8 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -551,9 +543,8 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -572,86 +563,76 @@
       <c r="F4" s="3">
         <v>5</v>
       </c>
-      <c r="G4" s="3">
-        <v>6</v>
+      <c r="G4" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3">
         <v>25</v>
       </c>
-      <c r="I5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="H5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
         <v>25</v>
       </c>
-      <c r="I6" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3">
         <v>25</v>
       </c>
-      <c r="I7" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="H7" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -663,18 +644,15 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="3">
+      <c r="F8" s="5"/>
+      <c r="G8" s="3">
         <v>25</v>
       </c>
-      <c r="I8" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="H8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -685,9 +663,8 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -696,9 +673,8 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -711,14 +687,13 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="6"/>
@@ -726,14 +701,13 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>2</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="6"/>
@@ -741,14 +715,13 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>3</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="6"/>
@@ -756,14 +729,13 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="6"/>
@@ -771,27 +743,18 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>5</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>6</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>18</v>
+      <c r="B16" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>